<commit_message>
Added excel document to track how algorithm scales
</commit_message>
<xml_diff>
--- a/How Hungarian Scales.xlsx
+++ b/How Hungarian Scales.xlsx
@@ -32,19 +32,19 @@
     <t>Sample Size (# teachers)</t>
   </si>
   <si>
-    <t>Log base 2</t>
+    <t>Square root</t>
   </si>
   <si>
-    <t>Log base 3</t>
+    <t>Cube root</t>
   </si>
   <si>
-    <t>Log base 4</t>
+    <t>Fourth root</t>
   </si>
   <si>
-    <t>Log base 5</t>
+    <t>Fifth root</t>
   </si>
   <si>
-    <t>Log base 6</t>
+    <t>Sixth root</t>
   </si>
 </sst>
 </file>
@@ -158,6 +158,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -268,64 +269,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>-3.7178567712185022</c:v>
+                  <c:v>0.27568097504180444</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.5311560570253624</c:v>
+                  <c:v>0.41593268686170842</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.4111954329844496</c:v>
+                  <c:v>0.61318838867023562</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.8287931725818577</c:v>
+                  <c:v>0.75033325929216277</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-6.7938828656575564E-2</c:v>
+                  <c:v>0.97672923576598236</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.87105507508662938</c:v>
+                  <c:v>1.3524052647043341</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5767639776731257</c:v>
+                  <c:v>1.7271363582531636</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.0617761975866897</c:v>
+                  <c:v>2.0432816741702551</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.7178683127326626</c:v>
+                  <c:v>2.5649561399758865</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.2567087675843793</c:v>
+                  <c:v>3.0916015267171804</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.6798741477466232</c:v>
+                  <c:v>3.5799441336423117</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.1614846386416593</c:v>
+                  <c:v>4.2302482196674935</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.4067407337205724</c:v>
+                  <c:v>4.6055401420463156</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.8064271770098781</c:v>
+                  <c:v>5.2898015085634356</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.0709903256259334</c:v>
+                  <c:v>5.7977581874376236</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.4246534048984509</c:v>
+                  <c:v>6.5537775366577709</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.728573602559365</c:v>
+                  <c:v>7.2817580294871105</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.0385020285760369</c:v>
+                  <c:v>8.1074656952712409</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.268172361031036</c:v>
+                  <c:v>8.7791799161425086</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.7144378641820923</c:v>
+                  <c:v>10.247633873241178</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -371,13 +372,14 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.12947148319551985"/>
-                  <c:y val="-7.9579104530669558E-3"/>
+                  <c:x val="-4.1589717719825413E-3"/>
+                  <c:y val="-2.7570549166681477E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -486,64 +488,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>-2.3457064564788634</c:v>
+                  <c:v>0.4235823584254893</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.5969816673099138</c:v>
+                  <c:v>0.55720546555426231</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.89036518677404497</c:v>
+                  <c:v>0.72176521602773891</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.52291027213877783</c:v>
+                  <c:v>0.82572632699276249</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4.2864628422226686E-2</c:v>
+                  <c:v>0.98442535645643492</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.54957456387157433</c:v>
+                  <c:v>1.2229383620653298</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.99482730787365614</c:v>
+                  <c:v>1.4395201590538196</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3008359482628666</c:v>
+                  <c:v>1.610221025941873</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.7147839847920916</c:v>
+                  <c:v>1.8737858806572765</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.0547544601860168</c:v>
+                  <c:v>2.1222131865315044</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.321742089211754</c:v>
+                  <c:v>2.340188457317911</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.6256044775495875</c:v>
+                  <c:v>2.615635567260457</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.7803438451796239</c:v>
+                  <c:v>2.7681336069915963</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.0325179143499978</c:v>
+                  <c:v>3.0359381347538044</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.1994386765104146</c:v>
+                  <c:v>3.2273054044409122</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.4225752359631465</c:v>
+                  <c:v>3.502093985052996</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.614327531378736</c:v>
+                  <c:v>3.7568526551886623</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.809870596830224</c:v>
+                  <c:v>4.0357421730020482</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.9547764430887313</c:v>
+                  <c:v>4.2556832847967501</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.2363386270192702</c:v>
+                  <c:v>4.7179036462863353</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -589,13 +591,14 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.16661168746664326"/>
-                  <c:y val="3.0974683469306744E-4"/>
+                  <c:x val="0.10552526338107458"/>
+                  <c:y val="-4.1593525414289352E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -704,64 +707,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>-1.8589283856092511</c:v>
+                  <c:v>0.52505330685731744</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.2655780285126812</c:v>
+                  <c:v>0.64492843545753853</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.7055977164922248</c:v>
+                  <c:v>0.78306346401184856</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.41439658629092885</c:v>
+                  <c:v>0.86621778975738128</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.3969414328287782E-2</c:v>
+                  <c:v>0.98829612756803942</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.43552753754331469</c:v>
+                  <c:v>1.1629296043631936</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.78838198883656285</c:v>
+                  <c:v>1.3142055996887108</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0308880987933449</c:v>
+                  <c:v>1.4294340398109509</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3589341563663313</c:v>
+                  <c:v>1.6015480448540675</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.6283543837921897</c:v>
+                  <c:v>1.7582950624730709</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.8399370738733116</c:v>
+                  <c:v>1.8920740296411005</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.0807423193208296</c:v>
+                  <c:v>2.0567567235012247</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.2033703668602862</c:v>
+                  <c:v>2.1460522225813414</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.403213588504939</c:v>
+                  <c:v>2.2999568492829243</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.5354951628129667</c:v>
+                  <c:v>2.4078534397752747</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.7123267024492255</c:v>
+                  <c:v>2.5600346748936373</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.8642868012796825</c:v>
+                  <c:v>2.6984732775195512</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.0192510142880185</c:v>
+                  <c:v>2.8473611810360908</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.134086180515518</c:v>
+                  <c:v>2.9629680923260899</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.3572189320910462</c:v>
+                  <c:v>3.2011925704713828</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -807,13 +810,14 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.16661168746664326"/>
-                  <c:y val="3.5843657240361884E-2"/>
+                  <c:x val="0.11481031444885545"/>
+                  <c:y val="1.6169163956085624E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -922,64 +926,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>-1.6011937576382429</c:v>
+                  <c:v>0.59725902155151744</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.0901095785863042</c:v>
+                  <c:v>0.70405926938755414</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.60776879184663446</c:v>
+                  <c:v>0.82231378177043757</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.35694179092228212</c:v>
+                  <c:v>0.89145962622580899</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-2.9259660885351969E-2</c:v>
+                  <c:v>0.99062589196878192</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.37514300163067049</c:v>
+                  <c:v>1.1283471624808508</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.67907528279837415</c:v>
+                  <c:v>1.2443159001490802</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.8879586762942836</c:v>
+                  <c:v>1.3308567019359698</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.1705221702244435</c:v>
+                  <c:v>1.4575785794094989</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.4025881226706822</c:v>
+                  <c:v>1.5706282523208583</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.5848355320947765</c:v>
+                  <c:v>1.6655224834251128</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.792253880645488</c:v>
+                  <c:v>1.7805178854044506</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.897879931520595</c:v>
+                  <c:v>1.8420958697058181</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.0700155132250293</c:v>
+                  <c:v>1.9470439304076843</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.1839566594640516</c:v>
+                  <c:v>2.0197798682700991</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.3362710571627772</c:v>
+                  <c:v>2.1212735567345615</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.4671623618203649</c:v>
+                  <c:v>2.2125571503850079</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.6006412695863292</c:v>
+                  <c:v>2.3096918819098584</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.69955489785962</c:v>
+                  <c:v>2.3844135422355222</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.8917509887436084</c:v>
+                  <c:v>2.5365851184947101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1025,13 +1029,14 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.0946344102530358E-2"/>
-                  <c:y val="9.4702191571426036E-2"/>
+                  <c:x val="-6.5319676266093474E-2"/>
+                  <c:y val="0.10563030636971733"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1140,64 +1145,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>-1.4382633288418263</c:v>
+                  <c:v>0.65083205085912088</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.97918482620897496</c:v>
+                  <c:v>0.74646196524287989</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.54592491480659877</c:v>
+                  <c:v>0.84956766418440088</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.32062096543011354</c:v>
+                  <c:v>0.90869484811611123</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-2.6282326586022777E-2</c:v>
+                  <c:v>0.99218211859337335</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.336970101053157</c:v>
+                  <c:v>1.1058654357856248</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.60997557110915068</c:v>
+                  <c:v>1.1998000496140262</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.7976039099257699</c:v>
+                  <c:v>1.2689448474783578</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0514149864744375</c:v>
+                  <c:v>1.3688629882706582</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.2598669290853612</c:v>
+                  <c:v>1.4567817909802085</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.4235696443255974</c:v>
+                  <c:v>1.5297674520390054</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.6098820147219479</c:v>
+                  <c:v>1.6172926659267508</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.704760023594607</c:v>
+                  <c:v>1.663770899791073</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.8593798461946642</c:v>
+                  <c:v>1.7423943683201586</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.9617268429275945</c:v>
+                  <c:v>1.7964702626096856</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.0985423979593798</c:v>
+                  <c:v>1.8713882507520978</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.2161147795997813</c:v>
+                  <c:v>1.9382602134875138</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.3360114612461138</c:v>
+                  <c:v>2.0089156709533751</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.4248600740948207</c:v>
+                  <c:v>2.0629307513333428</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.5974991367607418</c:v>
+                  <c:v>2.172073582152855</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1212,11 +1217,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="332851360"/>
-        <c:axId val="332862728"/>
+        <c:axId val="226624304"/>
+        <c:axId val="226624696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="332851360"/>
+        <c:axId val="226624304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1273,12 +1278,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332862728"/>
+        <c:crossAx val="226624696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="332862728"/>
+        <c:axId val="226624696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1335,7 +1340,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332851360"/>
+        <c:crossAx val="226624304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1347,38 +1352,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1976,16 +1949,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2273,7 +2246,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2314,24 +2287,24 @@
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="C2">
-        <f>LOG(B2,2)</f>
-        <v>-3.7178567712185022</v>
+        <f>B2^(1/2)</f>
+        <v>0.27568097504180444</v>
       </c>
       <c r="D2">
-        <f>LOG(B2,3)</f>
-        <v>-2.3457064564788634</v>
+        <f>B2^(1/3)</f>
+        <v>0.4235823584254893</v>
       </c>
       <c r="E2">
-        <f>LOG(B2,4)</f>
-        <v>-1.8589283856092511</v>
+        <f>B2^(1/4)</f>
+        <v>0.52505330685731744</v>
       </c>
       <c r="F2">
-        <f>LOG(B2,5)</f>
-        <v>-1.6011937576382429</v>
+        <f>B2^(1/5)</f>
+        <v>0.59725902155151744</v>
       </c>
       <c r="G2">
-        <f>LOG(B2, 6)</f>
-        <v>-1.4382633288418263</v>
+        <f>B2^(1/6)</f>
+        <v>0.65083205085912088</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2342,24 +2315,24 @@
         <v>0.17299999999999999</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C21" si="0">LOG(B3,2)</f>
-        <v>-2.5311560570253624</v>
+        <f t="shared" ref="C3:C21" si="0">B3^(1/2)</f>
+        <v>0.41593268686170842</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D21" si="1">LOG(B3,3)</f>
-        <v>-1.5969816673099138</v>
+        <f t="shared" ref="D3:D21" si="1">B3^(1/3)</f>
+        <v>0.55720546555426231</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E21" si="2">LOG(B3,4)</f>
-        <v>-1.2655780285126812</v>
+        <f t="shared" ref="E3:E21" si="2">B3^(1/4)</f>
+        <v>0.64492843545753853</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F21" si="3">LOG(B3,5)</f>
-        <v>-1.0901095785863042</v>
+        <f t="shared" ref="F3:F21" si="3">B3^(1/5)</f>
+        <v>0.70405926938755414</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G21" si="4">LOG(B3, 6)</f>
-        <v>-0.97918482620897496</v>
+        <f t="shared" ref="G3:G21" si="4">B3^(1/6)</f>
+        <v>0.74646196524287989</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2371,23 +2344,23 @@
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>-1.4111954329844496</v>
+        <v>0.61318838867023562</v>
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>-0.89036518677404497</v>
+        <v>0.72176521602773891</v>
       </c>
       <c r="E4">
         <f t="shared" si="2"/>
-        <v>-0.7055977164922248</v>
+        <v>0.78306346401184856</v>
       </c>
       <c r="F4">
         <f t="shared" si="3"/>
-        <v>-0.60776879184663446</v>
+        <v>0.82231378177043757</v>
       </c>
       <c r="G4">
         <f t="shared" si="4"/>
-        <v>-0.54592491480659877</v>
+        <v>0.84956766418440088</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2399,23 +2372,23 @@
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>-0.8287931725818577</v>
+        <v>0.75033325929216277</v>
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>-0.52291027213877783</v>
+        <v>0.82572632699276249</v>
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
-        <v>-0.41439658629092885</v>
+        <v>0.86621778975738128</v>
       </c>
       <c r="F5">
         <f t="shared" si="3"/>
-        <v>-0.35694179092228212</v>
+        <v>0.89145962622580899</v>
       </c>
       <c r="G5">
         <f t="shared" si="4"/>
-        <v>-0.32062096543011354</v>
+        <v>0.90869484811611123</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2427,23 +2400,23 @@
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>-6.7938828656575564E-2</v>
+        <v>0.97672923576598236</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>-4.2864628422226686E-2</v>
+        <v>0.98442535645643492</v>
       </c>
       <c r="E6">
         <f t="shared" si="2"/>
-        <v>-3.3969414328287782E-2</v>
+        <v>0.98829612756803942</v>
       </c>
       <c r="F6">
         <f t="shared" si="3"/>
-        <v>-2.9259660885351969E-2</v>
+        <v>0.99062589196878192</v>
       </c>
       <c r="G6">
         <f t="shared" si="4"/>
-        <v>-2.6282326586022777E-2</v>
+        <v>0.99218211859337335</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2455,23 +2428,23 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0.87105507508662938</v>
+        <v>1.3524052647043341</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>0.54957456387157433</v>
+        <v>1.2229383620653298</v>
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
-        <v>0.43552753754331469</v>
+        <v>1.1629296043631936</v>
       </c>
       <c r="F7">
         <f t="shared" si="3"/>
-        <v>0.37514300163067049</v>
+        <v>1.1283471624808508</v>
       </c>
       <c r="G7">
         <f t="shared" si="4"/>
-        <v>0.336970101053157</v>
+        <v>1.1058654357856248</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2483,23 +2456,23 @@
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>1.5767639776731257</v>
+        <v>1.7271363582531636</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>0.99482730787365614</v>
+        <v>1.4395201590538196</v>
       </c>
       <c r="E8">
         <f t="shared" si="2"/>
-        <v>0.78838198883656285</v>
+        <v>1.3142055996887108</v>
       </c>
       <c r="F8">
         <f t="shared" si="3"/>
-        <v>0.67907528279837415</v>
+        <v>1.2443159001490802</v>
       </c>
       <c r="G8">
         <f t="shared" si="4"/>
-        <v>0.60997557110915068</v>
+        <v>1.1998000496140262</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2511,23 +2484,23 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>2.0617761975866897</v>
+        <v>2.0432816741702551</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>1.3008359482628666</v>
+        <v>1.610221025941873</v>
       </c>
       <c r="E9">
         <f t="shared" si="2"/>
-        <v>1.0308880987933449</v>
+        <v>1.4294340398109509</v>
       </c>
       <c r="F9">
         <f t="shared" si="3"/>
-        <v>0.8879586762942836</v>
+        <v>1.3308567019359698</v>
       </c>
       <c r="G9">
         <f t="shared" si="4"/>
-        <v>0.7976039099257699</v>
+        <v>1.2689448474783578</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2539,23 +2512,23 @@
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>2.7178683127326626</v>
+        <v>2.5649561399758865</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>1.7147839847920916</v>
+        <v>1.8737858806572765</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>1.3589341563663313</v>
+        <v>1.6015480448540675</v>
       </c>
       <c r="F10">
         <f t="shared" si="3"/>
-        <v>1.1705221702244435</v>
+        <v>1.4575785794094989</v>
       </c>
       <c r="G10">
         <f t="shared" si="4"/>
-        <v>1.0514149864744375</v>
+        <v>1.3688629882706582</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2567,23 +2540,23 @@
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>3.2567087675843793</v>
+        <v>3.0916015267171804</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>2.0547544601860168</v>
+        <v>2.1222131865315044</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>1.6283543837921897</v>
+        <v>1.7582950624730709</v>
       </c>
       <c r="F11">
         <f t="shared" si="3"/>
-        <v>1.4025881226706822</v>
+        <v>1.5706282523208583</v>
       </c>
       <c r="G11">
         <f t="shared" si="4"/>
-        <v>1.2598669290853612</v>
+        <v>1.4567817909802085</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2595,23 +2568,23 @@
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>3.6798741477466232</v>
+        <v>3.5799441336423117</v>
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>2.321742089211754</v>
+        <v>2.340188457317911</v>
       </c>
       <c r="E12">
         <f t="shared" si="2"/>
-        <v>1.8399370738733116</v>
+        <v>1.8920740296411005</v>
       </c>
       <c r="F12">
         <f t="shared" si="3"/>
-        <v>1.5848355320947765</v>
+        <v>1.6655224834251128</v>
       </c>
       <c r="G12">
         <f t="shared" si="4"/>
-        <v>1.4235696443255974</v>
+        <v>1.5297674520390054</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2623,23 +2596,23 @@
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>4.1614846386416593</v>
+        <v>4.2302482196674935</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>2.6256044775495875</v>
+        <v>2.615635567260457</v>
       </c>
       <c r="E13">
         <f t="shared" si="2"/>
-        <v>2.0807423193208296</v>
+        <v>2.0567567235012247</v>
       </c>
       <c r="F13">
         <f t="shared" si="3"/>
-        <v>1.792253880645488</v>
+        <v>1.7805178854044506</v>
       </c>
       <c r="G13">
         <f t="shared" si="4"/>
-        <v>1.6098820147219479</v>
+        <v>1.6172926659267508</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2651,23 +2624,23 @@
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>4.4067407337205724</v>
+        <v>4.6055401420463156</v>
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>2.7803438451796239</v>
+        <v>2.7681336069915963</v>
       </c>
       <c r="E14">
         <f t="shared" si="2"/>
-        <v>2.2033703668602862</v>
+        <v>2.1460522225813414</v>
       </c>
       <c r="F14">
         <f t="shared" si="3"/>
-        <v>1.897879931520595</v>
+        <v>1.8420958697058181</v>
       </c>
       <c r="G14">
         <f t="shared" si="4"/>
-        <v>1.704760023594607</v>
+        <v>1.663770899791073</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2679,23 +2652,23 @@
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>4.8064271770098781</v>
+        <v>5.2898015085634356</v>
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
-        <v>3.0325179143499978</v>
+        <v>3.0359381347538044</v>
       </c>
       <c r="E15">
         <f t="shared" si="2"/>
-        <v>2.403213588504939</v>
+        <v>2.2999568492829243</v>
       </c>
       <c r="F15">
         <f t="shared" si="3"/>
-        <v>2.0700155132250293</v>
+        <v>1.9470439304076843</v>
       </c>
       <c r="G15">
         <f t="shared" si="4"/>
-        <v>1.8593798461946642</v>
+        <v>1.7423943683201586</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2707,23 +2680,23 @@
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>5.0709903256259334</v>
+        <v>5.7977581874376236</v>
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
-        <v>3.1994386765104146</v>
+        <v>3.2273054044409122</v>
       </c>
       <c r="E16">
         <f t="shared" si="2"/>
-        <v>2.5354951628129667</v>
+        <v>2.4078534397752747</v>
       </c>
       <c r="F16">
         <f t="shared" si="3"/>
-        <v>2.1839566594640516</v>
+        <v>2.0197798682700991</v>
       </c>
       <c r="G16">
         <f t="shared" si="4"/>
-        <v>1.9617268429275945</v>
+        <v>1.7964702626096856</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2735,23 +2708,23 @@
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>5.4246534048984509</v>
+        <v>6.5537775366577709</v>
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
-        <v>3.4225752359631465</v>
+        <v>3.502093985052996</v>
       </c>
       <c r="E17">
         <f t="shared" si="2"/>
-        <v>2.7123267024492255</v>
+        <v>2.5600346748936373</v>
       </c>
       <c r="F17">
         <f t="shared" si="3"/>
-        <v>2.3362710571627772</v>
+        <v>2.1212735567345615</v>
       </c>
       <c r="G17">
         <f t="shared" si="4"/>
-        <v>2.0985423979593798</v>
+        <v>1.8713882507520978</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2763,23 +2736,23 @@
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>5.728573602559365</v>
+        <v>7.2817580294871105</v>
       </c>
       <c r="D18">
         <f t="shared" si="1"/>
-        <v>3.614327531378736</v>
+        <v>3.7568526551886623</v>
       </c>
       <c r="E18">
         <f t="shared" si="2"/>
-        <v>2.8642868012796825</v>
+        <v>2.6984732775195512</v>
       </c>
       <c r="F18">
         <f t="shared" si="3"/>
-        <v>2.4671623618203649</v>
+        <v>2.2125571503850079</v>
       </c>
       <c r="G18">
         <f t="shared" si="4"/>
-        <v>2.2161147795997813</v>
+        <v>1.9382602134875138</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2791,23 +2764,23 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>6.0385020285760369</v>
+        <v>8.1074656952712409</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
-        <v>3.809870596830224</v>
+        <v>4.0357421730020482</v>
       </c>
       <c r="E19">
         <f t="shared" si="2"/>
-        <v>3.0192510142880185</v>
+        <v>2.8473611810360908</v>
       </c>
       <c r="F19">
         <f t="shared" si="3"/>
-        <v>2.6006412695863292</v>
+        <v>2.3096918819098584</v>
       </c>
       <c r="G19">
         <f t="shared" si="4"/>
-        <v>2.3360114612461138</v>
+        <v>2.0089156709533751</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2819,23 +2792,23 @@
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>6.268172361031036</v>
+        <v>8.7791799161425086</v>
       </c>
       <c r="D20">
         <f t="shared" si="1"/>
-        <v>3.9547764430887313</v>
+        <v>4.2556832847967501</v>
       </c>
       <c r="E20">
         <f t="shared" si="2"/>
-        <v>3.134086180515518</v>
+        <v>2.9629680923260899</v>
       </c>
       <c r="F20">
         <f t="shared" si="3"/>
-        <v>2.69955489785962</v>
+        <v>2.3844135422355222</v>
       </c>
       <c r="G20">
         <f t="shared" si="4"/>
-        <v>2.4248600740948207</v>
+        <v>2.0629307513333428</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2847,23 +2820,23 @@
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>6.7144378641820923</v>
+        <v>10.247633873241178</v>
       </c>
       <c r="D21">
         <f t="shared" si="1"/>
-        <v>4.2363386270192702</v>
+        <v>4.7179036462863353</v>
       </c>
       <c r="E21">
         <f t="shared" si="2"/>
-        <v>3.3572189320910462</v>
+        <v>3.2011925704713828</v>
       </c>
       <c r="F21">
         <f t="shared" si="3"/>
-        <v>2.8917509887436084</v>
+        <v>2.5365851184947101</v>
       </c>
       <c r="G21">
         <f t="shared" si="4"/>
-        <v>2.5974991367607418</v>
+        <v>2.172073582152855</v>
       </c>
     </row>
   </sheetData>

</xml_diff>